<commit_message>
Clean up, two bugs fixed
</commit_message>
<xml_diff>
--- a/test_result_rows_added.xlsx
+++ b/test_result_rows_added.xlsx
@@ -51,13 +51,16 @@
     <t>Summary. Do not remove but push down</t>
   </si>
   <si>
-    <t>t</t>
+    <t>link</t>
   </si>
   <si>
     <t>example</t>
   </si>
   <si>
     <t>ex1</t>
+  </si>
+  <si>
+    <t>link2</t>
   </si>
   <si>
     <t>ex3</t>
@@ -346,13 +349,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="9">

</xml_diff>